<commit_message>
Extended the GLCode Hierarchy to dirll down to the GLTransaction level
</commit_message>
<xml_diff>
--- a/Reports/TrialBalance_FromWarehouse_003.xlsx
+++ b/Reports/TrialBalance_FromWarehouse_003.xlsx
@@ -13,13 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Timeline_TransactionDate">#N/A</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="165" r:id="rId2"/>
+    <pivotCache cacheId="68" r:id="rId3"/>
+    <pivotCache cacheId="111" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,12 +29,12 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{A2CB5862-8E78-49c6-8D9D-AF26E26ADB89}">
       <x15:timelineCachePivotCaches>
-        <pivotCache cacheId="164" r:id="rId3"/>
+        <pivotCache cacheId="64" r:id="rId5"/>
       </x15:timelineCachePivotCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}">
       <x15:timelineCacheRefs>
-        <x15:timelineCacheRef r:id="rId4"/>
+        <x15:timelineCacheRef r:id="rId6"/>
       </x15:timelineCacheRefs>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Grand Total</t>
   </si>
@@ -61,9 +63,6 @@
   </si>
   <si>
     <t>20000 - 29999:  Liabilities</t>
-  </si>
-  <si>
-    <t>13000 - 13999:  Banks</t>
   </si>
   <si>
     <t>12100 - 12399:  Paga Receivables</t>
@@ -78,54 +77,6 @@
     <t>22000 - 22999:  Creditors - Pagatech Income</t>
   </si>
   <si>
-    <t>12110:  Debtors - Agent Accept Deposit Commission</t>
-  </si>
-  <si>
-    <t>12120:  Debtors - Agent Sign up Fees Commission</t>
-  </si>
-  <si>
-    <t>12130:  Debtors - Agent Dispense cash commission</t>
-  </si>
-  <si>
-    <t>12150:  Debtors - Promotional giveaways</t>
-  </si>
-  <si>
-    <t>12160:  Debtors - Agent Money Transfer Commission</t>
-  </si>
-  <si>
-    <t>12170:  Debtors - Agent Bill Pay Commission</t>
-  </si>
-  <si>
-    <t>12180:  Debtors - Agent Airtime Sale Commission</t>
-  </si>
-  <si>
-    <t>12190:  Debtors - Bank Transfer Processing Fees</t>
-  </si>
-  <si>
-    <t>12410:  Paga 3rd Party Funds Recievable</t>
-  </si>
-  <si>
-    <t>21010:  Creditors - Pagatech Pre-Paid Service Repayment</t>
-  </si>
-  <si>
-    <t>21020:  Creditors - Virtual Account</t>
-  </si>
-  <si>
-    <t>21030:  Creditors - Commission Payable</t>
-  </si>
-  <si>
-    <t>21040:  Creditors - Commission Accrued</t>
-  </si>
-  <si>
-    <t>21080:  Creditors - Transaction Processing Fees Payable</t>
-  </si>
-  <si>
-    <t>21090:  Creditors - Cash Bonus Account</t>
-  </si>
-  <si>
-    <t>22100:  Creditors - Pagatech Third Party Cash Transaction Commission Owed</t>
-  </si>
-  <si>
     <t>Debits</t>
   </si>
   <si>
@@ -135,43 +86,10 @@
     <t>Balance</t>
   </si>
   <si>
-    <t>13000 - 19999:  Other Assets</t>
-  </si>
-  <si>
     <t>Assets</t>
   </si>
   <si>
     <t>Liabilities</t>
-  </si>
-  <si>
-    <t>13110:  Pool Accounts</t>
-  </si>
-  <si>
-    <t>21070:  Creditors - Pagatech Third Party Invoiced Cash Payable</t>
-  </si>
-  <si>
-    <t>22010:  Creditors - Pagatech Money Transfer Fees</t>
-  </si>
-  <si>
-    <t>22020:  Creditors - Pagatech Airtime Sale Commission</t>
-  </si>
-  <si>
-    <t>22030:  Creditors - Pagatech Bill Pay Commission</t>
-  </si>
-  <si>
-    <t>22050:  Creditors - Pagatech Account Balance Fee</t>
-  </si>
-  <si>
-    <t>22070:  Creditors - Pagatech Withdrawals Fee</t>
-  </si>
-  <si>
-    <t>22080:  Creditors - Pagatech Load Cash Fee</t>
-  </si>
-  <si>
-    <t>22090:  Creditors - Pagatech Premium SMS Fee</t>
-  </si>
-  <si>
-    <t>22120:  Creditors - Fees Accrued</t>
   </si>
   <si>
     <t>Chart of Accounts</t>
@@ -180,23 +98,36 @@
     <t>General Ledger</t>
   </si>
   <si>
-    <t>2/27/2015 12:10:15 PM</t>
+    <t>3/4/2015 1:30:14 PM</t>
   </si>
   <si>
-    <t>Transactions Available Through</t>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>10100 - 19999:  Other Assets</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -236,27 +167,25 @@
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="18">
     <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" readingOrder="0"/>
@@ -268,7 +197,37 @@
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -294,12 +253,12 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" Requires="tsle">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
+      <mc:Choice Requires="tsle">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="Date"/>
@@ -311,12 +270,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
-              <tsle:timeslicer xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" name="Date"/>
+              <tsle:timeslicer name="Date"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -360,75 +319,12 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42062.814809837961" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42067.584773032409" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="10">
-    <cacheField name="[Measures].[Debits]" caption="Debits" numFmtId="0" hierarchy="291" level="32767"/>
-    <cacheField name="[Measures].[Credits]" caption="Credits" numFmtId="0" hierarchy="290" level="32767"/>
-    <cacheField name="[Measures].[Balance]" caption="Balance" numFmtId="0" hierarchy="292" level="32767"/>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[MainHeading]" caption="MainHeading" numFmtId="0" hierarchy="46" level="1">
-      <sharedItems count="1">
-        <s v="[GLCodeHierarchy].[GLCodes].[MainHeading].&amp;[Chart of Accounts]" c="Chart of Accounts"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_1]" caption="SubHeading_1" numFmtId="0" hierarchy="46" level="2">
-      <sharedItems count="2">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_1].&amp;[Assets]" c="Assets"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_1].&amp;[Liabilities]" c="Liabilities"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_2]" caption="SubHeading_2" numFmtId="0" hierarchy="46" level="3">
-      <sharedItems count="3">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;[12000 - 12999:  Receivables]" c="12000 - 12999:  Receivables"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;[13000 - 19999:  Other Assets]" c="13000 - 19999:  Other Assets"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;[20000 - 29999:  Liabilities]" c="20000 - 29999:  Liabilities"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_3]" caption="SubHeading_3" numFmtId="0" hierarchy="46" level="4">
-      <sharedItems count="5">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[12100 - 12399:  Paga Receivables]" c="12100 - 12399:  Paga Receivables"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[12400 - 12499:  Other Receivables]" c="12400 - 12499:  Other Receivables"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[13000 - 13999:  Banks]" c="13000 - 13999:  Banks"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[21000 - 21299:  Creditor Others]" c="21000 - 21299:  Creditor Others"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[22000 - 22999:  Creditors - Pagatech Income]" c="22000 - 22999:  Creditors - Pagatech Income"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_4]" caption="SubHeading_4" numFmtId="0" hierarchy="46" level="5">
-      <sharedItems count="26">
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12110:  Debtors - Agent Accept Deposit Commission]" c="12110:  Debtors - Agent Accept Deposit Commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12120:  Debtors - Agent Sign up Fees Commission]" c="12120:  Debtors - Agent Sign up Fees Commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12130:  Debtors - Agent Dispense cash commission]" c="12130:  Debtors - Agent Dispense cash commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12150:  Debtors - Promotional giveaways]" c="12150:  Debtors - Promotional giveaways"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12160:  Debtors - Agent Money Transfer Commission]" c="12160:  Debtors - Agent Money Transfer Commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12170:  Debtors - Agent Bill Pay Commission]" c="12170:  Debtors - Agent Bill Pay Commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12180:  Debtors - Agent Airtime Sale Commission]" c="12180:  Debtors - Agent Airtime Sale Commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12190:  Debtors - Bank Transfer Processing Fees]" c="12190:  Debtors - Bank Transfer Processing Fees"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[12410:  Paga 3rd Party Funds Recievable]" c="12410:  Paga 3rd Party Funds Recievable"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[13110:  Pool Accounts]" c="13110:  Pool Accounts"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[21010:  Creditors - Pagatech Pre-Paid Service Repayment]" c="21010:  Creditors - Pagatech Pre-Paid Service Repayment"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[21020:  Creditors - Virtual Account]" c="21020:  Creditors - Virtual Account"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[21030:  Creditors - Commission Payable]" c="21030:  Creditors - Commission Payable"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[21040:  Creditors - Commission Accrued]" c="21040:  Creditors - Commission Accrued"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[21080:  Creditors - Transaction Processing Fees Payable]" c="21080:  Creditors - Transaction Processing Fees Payable"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[21090:  Creditors - Cash Bonus Account]" c="21090:  Creditors - Cash Bonus Account"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22100:  Creditors - Pagatech Third Party Cash Transaction Commission Owed]" c="22100:  Creditors - Pagatech Third Party Cash Transaction Commission Owed"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[21070:  Creditors - Pagatech Third Party Invoiced Cash Payable]" c="21070:  Creditors - Pagatech Third Party Invoiced Cash Payable"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22010:  Creditors - Pagatech Money Transfer Fees]" c="22010:  Creditors - Pagatech Money Transfer Fees"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22020:  Creditors - Pagatech Airtime Sale Commission]" c="22020:  Creditors - Pagatech Airtime Sale Commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22030:  Creditors - Pagatech Bill Pay Commission]" c="22030:  Creditors - Pagatech Bill Pay Commission"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22050:  Creditors - Pagatech Account Balance Fee]" c="22050:  Creditors - Pagatech Account Balance Fee"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22070:  Creditors - Pagatech Withdrawals Fee]" c="22070:  Creditors - Pagatech Withdrawals Fee"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22080:  Creditors - Pagatech Load Cash Fee]" c="22080:  Creditors - Pagatech Load Cash Fee"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22090:  Creditors - Pagatech Premium SMS Fee]" c="22090:  Creditors - Pagatech Premium SMS Fee"/>
-        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_4].&amp;[22120:  Creditors - Fees Accrued]" c="22120:  Creditors - Fees Accrued"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[TransactionDate].[Date].[Date]" caption="Date" numFmtId="0" hierarchy="233" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
+  <cacheFields count="1">
     <cacheField name="[LatestFinancialTransaction].[TransactionTime].[TransactionTime]" caption="TransactionTime" numFmtId="0" hierarchy="71" level="1">
       <sharedItems count="1">
-        <s v="[LatestFinancialTransaction].[TransactionTime].&amp;[2015-02-27T12:10:15]" c="2/27/2015 12:10:15 PM"/>
+        <s v="[LatestFinancialTransaction].[TransactionTime].&amp;[2015-03-04T13:30:14]" c="3/4/2015 1:30:14 PM"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -444,6 +340,501 @@
     <cacheHierarchy uniqueName="[FinancialAccount].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[FinancialAccount].[RestrictedBalance].[All]" allUniqueName="[FinancialAccount].[RestrictedBalance].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialAccount].[TotalBalance]" caption="TotalBalance" attribute="1" defaultMemberUniqueName="[FinancialAccount].[TotalBalance].[All]" allUniqueName="[FinancialAccount].[TotalBalance].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[Cancelled]" caption="Cancelled" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[Cancelled].[All]" allUniqueName="[FinancialTransaction].[Cancelled].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[DimCurrencyID]" caption="DimCurrencyID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimCurrencyID].[All]" allUniqueName="[FinancialTransaction].[DimCurrencyID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[DimEffectiveDateID]" caption="DimEffectiveDateID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimEffectiveDateID].[All]" allUniqueName="[FinancialTransaction].[DimEffectiveDateID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[DimEffectiveTimeID]" caption="DimEffectiveTimeID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimEffectiveTimeID].[All]" allUniqueName="[FinancialTransaction].[DimEffectiveTimeID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[DimFinancialTxDateID]" caption="DimFinancialTxDateID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimFinancialTxDateID].[All]" allUniqueName="[FinancialTransaction].[DimFinancialTxDateID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[DimFinancialTxTimeID]" caption="DimFinancialTxTimeID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimFinancialTxTimeID].[All]" allUniqueName="[FinancialTransaction].[DimFinancialTxTimeID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[DimFinancialTxTypeID]" caption="DimFinancialTxTypeID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimFinancialTxTypeID].[All]" allUniqueName="[FinancialTransaction].[DimFinancialTxTypeID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[DimUserID]" caption="DimUserID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimUserID].[All]" allUniqueName="[FinancialTransaction].[DimUserID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[ExchangeRate]" caption="ExchangeRate" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ExchangeRate].[All]" allUniqueName="[FinancialTransaction].[ExchangeRate].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[ExternalReferenceNumber]" caption="ExternalReferenceNumber" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ExternalReferenceNumber].[All]" allUniqueName="[FinancialTransaction].[ExternalReferenceNumber].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[FactFinancialTxID]" caption="FactFinancialTxID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[FactFinancialTxID].[All]" allUniqueName="[FinancialTransaction].[FactFinancialTxID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[FactIntegrationTxID]" caption="FactIntegrationTxID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[FactIntegrationTxID].[All]" allUniqueName="[FinancialTransaction].[FactIntegrationTxID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[FactOriginalFinancialTxID]" caption="FactOriginalFinancialTxID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[FactOriginalFinancialTxID].[All]" allUniqueName="[FinancialTransaction].[FactOriginalFinancialTxID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[FactProcessEventID]" caption="FactProcessEventID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[FactProcessEventID].[All]" allUniqueName="[FinancialTransaction].[FactProcessEventID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[FactRelatedFinancialTxID]" caption="FactRelatedFinancialTxID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[FactRelatedFinancialTxID].[All]" allUniqueName="[FinancialTransaction].[FactRelatedFinancialTxID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[FinancialTx_Amount]" caption="FinancialTx_Amount" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[FinancialTx_Amount].[All]" allUniqueName="[FinancialTransaction].[FinancialTx_Amount].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[FinancialTx_Fee]" caption="FinancialTx_Fee" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[FinancialTx_Fee].[All]" allUniqueName="[FinancialTransaction].[FinancialTx_Fee].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[ForeignCurrencyAmount]" caption="ForeignCurrencyAmount" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ForeignCurrencyAmount].[All]" allUniqueName="[FinancialTransaction].[ForeignCurrencyAmount].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[IsIntegrationTx]" caption="IsIntegrationTx" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[IsIntegrationTx].[All]" allUniqueName="[FinancialTransaction].[IsIntegrationTx].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[ReferenceNumber]" caption="ReferenceNumber" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ReferenceNumber].[All]" allUniqueName="[FinancialTransaction].[ReferenceNumber].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[Reversed]" caption="Reversed" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[Reversed].[All]" allUniqueName="[FinancialTransaction].[Reversed].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[ShortCode]" caption="ShortCode" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ShortCode].[All]" allUniqueName="[FinancialTransaction].[ShortCode].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[SourceKey].[All]" allUniqueName="[FinancialTransaction].[SourceKey].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[TextDescription]" caption="TextDescription" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[TextDescription].[All]" allUniqueName="[FinancialTransaction].[TextDescription].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTransactionType]" caption="FinancialTransactionType" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" allUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[ForUser].[DimCreatedDateID].[All]" allUniqueName="[ForUser].[DimCreatedDateID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[ForUser].[DimDateOfBirthID].[All]" allUniqueName="[ForUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[DimForUserID]" caption="DimForUserID" attribute="1" defaultMemberUniqueName="[ForUser].[DimForUserID].[All]" allUniqueName="[ForUser].[DimForUserID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[FirstName]" caption="FirstName" attribute="1" defaultMemberUniqueName="[ForUser].[FirstName].[All]" allUniqueName="[ForUser].[FirstName].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[ForUser].[Gender].[All]" allUniqueName="[ForUser].[Gender].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[IsEnabled]" caption="IsEnabled" attribute="1" defaultMemberUniqueName="[ForUser].[IsEnabled].[All]" allUniqueName="[ForUser].[IsEnabled].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[LastName]" caption="LastName" attribute="1" defaultMemberUniqueName="[ForUser].[LastName].[All]" allUniqueName="[ForUser].[LastName].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[MiddleName]" caption="MiddleName" attribute="1" defaultMemberUniqueName="[ForUser].[MiddleName].[All]" allUniqueName="[ForUser].[MiddleName].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[ForUser].[Name].[All]" allUniqueName="[ForUser].[Name].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[RoleName]" caption="RoleName" attribute="1" defaultMemberUniqueName="[ForUser].[RoleName].[All]" allUniqueName="[ForUser].[RoleName].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ForUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[ForUser].[SourceKey].[All]" allUniqueName="[ForUser].[SourceKey].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[GLCodes]" caption="GLCodes" defaultMemberUniqueName="[GLCodeHierarchy].[GLCodes].[All]" allUniqueName="[GLCodeHierarchy].[GLCodes].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[CreditAmount]" caption="CreditAmount" attribute="1" defaultMemberUniqueName="[GLTransaction].[CreditAmount].[All]" allUniqueName="[GLTransaction].[CreditAmount].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[DebitAmount]" caption="DebitAmount" attribute="1" defaultMemberUniqueName="[GLTransaction].[DebitAmount].[All]" allUniqueName="[GLTransaction].[DebitAmount].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[DimFinancialAccountID]" caption="DimFinancialAccountID" attribute="1" defaultMemberUniqueName="[GLTransaction].[DimFinancialAccountID].[All]" allUniqueName="[GLTransaction].[DimFinancialAccountID].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[DimGLCodeID]" caption="DimGLCodeID" attribute="1" defaultMemberUniqueName="[GLTransaction].[DimGLCodeID].[All]" allUniqueName="[GLTransaction].[DimGLCodeID].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[FactFinancialTxID]" caption="FactFinancialTxID" attribute="1" defaultMemberUniqueName="[GLTransaction].[FactFinancialTxID].[All]" allUniqueName="[GLTransaction].[FactFinancialTxID].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[FactGLTxID]" caption="FactGLTxID" attribute="1" defaultMemberUniqueName="[GLTransaction].[FactGLTxID].[All]" allUniqueName="[GLTransaction].[FactGLTxID].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[FinancialTransactionID]" caption="FinancialTransactionID" attribute="1" defaultMemberUniqueName="[GLTransaction].[FinancialTransactionID].[All]" allUniqueName="[GLTransaction].[FinancialTransactionID].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[Movement]" caption="Movement" attribute="1" defaultMemberUniqueName="[GLTransaction].[Movement].[All]" allUniqueName="[GLTransaction].[Movement].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[GLTransaction].[SourceKey].[All]" allUniqueName="[GLTransaction].[SourceKey].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[TextDescription]" caption="TextDescription" attribute="1" defaultMemberUniqueName="[GLTransaction].[TextDescription].[All]" allUniqueName="[GLTransaction].[TextDescription].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[TransactionLineNumber]" caption="TransactionLineNumber" attribute="1" defaultMemberUniqueName="[GLTransaction].[TransactionLineNumber].[All]" allUniqueName="[GLTransaction].[TransactionLineNumber].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[InitiatingUser].[DimCreatedDateID].[All]" allUniqueName="[InitiatingUser].[DimCreatedDateID].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[InitiatingUser].[DimDateOfBirthID].[All]" allUniqueName="[InitiatingUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[DimInitiatingUserID]" caption="DimInitiatingUserID" attribute="1" defaultMemberUniqueName="[InitiatingUser].[DimInitiatingUserID].[All]" allUniqueName="[InitiatingUser].[DimInitiatingUserID].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[FirstName]" caption="FirstName" attribute="1" defaultMemberUniqueName="[InitiatingUser].[FirstName].[All]" allUniqueName="[InitiatingUser].[FirstName].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[InitiatingUser].[Gender].[All]" allUniqueName="[InitiatingUser].[Gender].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[IsEnabled]" caption="IsEnabled" attribute="1" defaultMemberUniqueName="[InitiatingUser].[IsEnabled].[All]" allUniqueName="[InitiatingUser].[IsEnabled].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[LastName]" caption="LastName" attribute="1" defaultMemberUniqueName="[InitiatingUser].[LastName].[All]" allUniqueName="[InitiatingUser].[LastName].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[MiddleName]" caption="MiddleName" attribute="1" defaultMemberUniqueName="[InitiatingUser].[MiddleName].[All]" allUniqueName="[InitiatingUser].[MiddleName].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[InitiatingUser].[Name].[All]" allUniqueName="[InitiatingUser].[Name].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[RoleName]" caption="RoleName" attribute="1" defaultMemberUniqueName="[InitiatingUser].[RoleName].[All]" allUniqueName="[InitiatingUser].[RoleName].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[InitiatingUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[InitiatingUser].[SourceKey].[All]" allUniqueName="[InitiatingUser].[SourceKey].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[LatestFinancialTransaction].[FactFinancialTxID]" caption="FactFinancialTxID" attribute="1" defaultMemberUniqueName="[LatestFinancialTransaction].[FactFinancialTxID].[All]" allUniqueName="[LatestFinancialTransaction].[FactFinancialTxID].[All]" dimensionUniqueName="[LatestFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[LatestFinancialTransaction].[TransactionDate]" caption="TransactionDate" attribute="1" defaultMemberUniqueName="[LatestFinancialTransaction].[TransactionDate].[All]" allUniqueName="[LatestFinancialTransaction].[TransactionDate].[All]" dimensionUniqueName="[LatestFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[LatestFinancialTransaction].[TransactionTime]" caption="TransactionTime" attribute="1" defaultMemberUniqueName="[LatestFinancialTransaction].[TransactionTime].[All]" allUniqueName="[LatestFinancialTransaction].[TransactionTime].[All]" dimensionUniqueName="[LatestFinancialTransaction]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Organization].[DimBusinessTypeID]" caption="DimBusinessTypeID" attribute="1" defaultMemberUniqueName="[Organization].[DimBusinessTypeID].[All]" allUniqueName="[Organization].[DimBusinessTypeID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[DimOrganizationID]" caption="DimOrganizationID" attribute="1" defaultMemberUniqueName="[Organization].[DimOrganizationID].[All]" allUniqueName="[Organization].[DimOrganizationID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[DimOrganizationSubscriptionStatusID]" caption="DimOrganizationSubscriptionStatusID" attribute="1" defaultMemberUniqueName="[Organization].[DimOrganizationSubscriptionStatusID].[All]" allUniqueName="[Organization].[DimOrganizationSubscriptionStatusID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[DimOrganizationVerificationStatusID]" caption="DimOrganizationVerificationStatusID" attribute="1" defaultMemberUniqueName="[Organization].[DimOrganizationVerificationStatusID].[All]" allUniqueName="[Organization].[DimOrganizationVerificationStatusID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[Organization].[DimPagaAccountID].[All]" allUniqueName="[Organization].[DimPagaAccountID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[DisplayName]" caption="DisplayName" attribute="1" defaultMemberUniqueName="[Organization].[DisplayName].[All]" allUniqueName="[Organization].[DisplayName].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[Organization]" caption="Organization" attribute="1" defaultMemberUniqueName="[Organization].[Organization].[All]" allUniqueName="[Organization].[Organization].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[OrganizationCode]" caption="OrganizationCode" attribute="1" defaultMemberUniqueName="[Organization].[OrganizationCode].[All]" allUniqueName="[Organization].[OrganizationCode].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[RcName]" caption="RcName" attribute="1" defaultMemberUniqueName="[Organization].[RcName].[All]" allUniqueName="[Organization].[RcName].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[ReferenceNumber]" caption="ReferenceNumber" attribute="1" defaultMemberUniqueName="[Organization].[ReferenceNumber].[All]" allUniqueName="[Organization].[ReferenceNumber].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Organization].[SourceKey].[All]" allUniqueName="[Organization].[SourceKey].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[TaxIDNumber]" caption="TaxIDNumber" attribute="1" defaultMemberUniqueName="[Organization].[TaxIDNumber].[All]" allUniqueName="[Organization].[TaxIDNumber].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[TextDesciption]" caption="TextDesciption" attribute="1" defaultMemberUniqueName="[Organization].[TextDesciption].[All]" allUniqueName="[Organization].[TextDesciption].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[VATCertificationNumber]" caption="VATCertificationNumber" attribute="1" defaultMemberUniqueName="[Organization].[VATCertificationNumber].[All]" allUniqueName="[Organization].[VATCertificationNumber].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Organization].[WebsiteURL]" caption="WebsiteURL" attribute="1" defaultMemberUniqueName="[Organization].[WebsiteURL].[All]" allUniqueName="[Organization].[WebsiteURL].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[BankingStatus]" caption="BankingStatus" attribute="1" defaultMemberUniqueName="[PagaAccount].[BankingStatus].[All]" allUniqueName="[PagaAccount].[BankingStatus].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[PagaAccount].[DimCreatedDateID].[All]" allUniqueName="[PagaAccount].[DimCreatedDateID].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[PagaAccount].[DimPagaAccountID].[All]" allUniqueName="[PagaAccount].[DimPagaAccountID].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[DimPagaAccountStatusID]" caption="DimPagaAccountStatusID" attribute="1" defaultMemberUniqueName="[PagaAccount].[DimPagaAccountStatusID].[All]" allUniqueName="[PagaAccount].[DimPagaAccountStatusID].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[DimRegistrationDateID]" caption="DimRegistrationDateID" attribute="1" defaultMemberUniqueName="[PagaAccount].[DimRegistrationDateID].[All]" allUniqueName="[PagaAccount].[DimRegistrationDateID].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[ExternalAccountNumber]" caption="ExternalAccountNumber" attribute="1" defaultMemberUniqueName="[PagaAccount].[ExternalAccountNumber].[All]" allUniqueName="[PagaAccount].[ExternalAccountNumber].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[hasOnlineAccount]" caption="hasOnlineAccount" attribute="1" defaultMemberUniqueName="[PagaAccount].[hasOnlineAccount].[All]" allUniqueName="[PagaAccount].[hasOnlineAccount].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsActivePagaAccount]" caption="IsActivePagaAccount" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsActivePagaAccount].[All]" allUniqueName="[PagaAccount].[IsActivePagaAccount].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsAffiliate]" caption="IsAffiliate" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsAffiliate].[All]" allUniqueName="[PagaAccount].[IsAffiliate].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsAgent]" caption="IsAgent" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsAgent].[All]" allUniqueName="[PagaAccount].[IsAgent].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsBank]" caption="IsBank" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsBank].[All]" allUniqueName="[PagaAccount].[IsBank].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsBusiness]" caption="IsBusiness" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsBusiness].[All]" allUniqueName="[PagaAccount].[IsBusiness].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsCardProcessor]" caption="IsCardProcessor" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsCardProcessor].[All]" allUniqueName="[PagaAccount].[IsCardProcessor].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsCashCollector]" caption="IsCashCollector" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsCashCollector].[All]" allUniqueName="[PagaAccount].[IsCashCollector].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsCustomer]" caption="IsCustomer" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsCustomer].[All]" allUniqueName="[PagaAccount].[IsCustomer].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsEnabled]" caption="IsEnabled" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsEnabled].[All]" allUniqueName="[PagaAccount].[IsEnabled].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsMerchant]" caption="IsMerchant" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsMerchant].[All]" allUniqueName="[PagaAccount].[IsMerchant].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsMobileOperator]" caption="IsMobileOperator" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsMobileOperator].[All]" allUniqueName="[PagaAccount].[IsMobileOperator].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsPaga]" caption="IsPaga" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsPaga].[All]" allUniqueName="[PagaAccount].[IsPaga].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsRemittanceProcessor]" caption="IsRemittanceProcessor" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsRemittanceProcessor].[All]" allUniqueName="[PagaAccount].[IsRemittanceProcessor].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[IsServiceAggregator]" caption="IsServiceAggregator" attribute="1" defaultMemberUniqueName="[PagaAccount].[IsServiceAggregator].[All]" allUniqueName="[PagaAccount].[IsServiceAggregator].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[PagaAccount].[Name].[All]" allUniqueName="[PagaAccount].[Name].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[PagaAccountNumber]" caption="PagaAccountNumber" attribute="1" defaultMemberUniqueName="[PagaAccount].[PagaAccountNumber].[All]" allUniqueName="[PagaAccount].[PagaAccountNumber].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccount].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[PagaAccount].[SourceKey].[All]" allUniqueName="[PagaAccount].[SourceKey].[All]" dimensionUniqueName="[PagaAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccountStatus].[DimPagaAccountStatusID]" caption="DimPagaAccountStatusID" attribute="1" defaultMemberUniqueName="[PagaAccountStatus].[DimPagaAccountStatusID].[All]" allUniqueName="[PagaAccountStatus].[DimPagaAccountStatusID].[All]" dimensionUniqueName="[PagaAccountStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccountStatus].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[PagaAccountStatus].[Name].[All]" allUniqueName="[PagaAccountStatus].[Name].[All]" dimensionUniqueName="[PagaAccountStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccountStatus].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[PagaAccountStatus].[SourceKey].[All]" allUniqueName="[PagaAccountStatus].[SourceKey].[All]" dimensionUniqueName="[PagaAccountStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccountUserType].[DimPagaAccountUserTypeID]" caption="DimPagaAccountUserTypeID" attribute="1" defaultMemberUniqueName="[PagaAccountUserType].[DimPagaAccountUserTypeID].[All]" allUniqueName="[PagaAccountUserType].[DimPagaAccountUserTypeID].[All]" dimensionUniqueName="[PagaAccountUserType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccountUserType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[PagaAccountUserType].[Name].[All]" allUniqueName="[PagaAccountUserType].[Name].[All]" dimensionUniqueName="[PagaAccountUserType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PagaAccountUserType].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[PagaAccountUserType].[SourceKey].[All]" allUniqueName="[PagaAccountUserType].[SourceKey].[All]" dimensionUniqueName="[PagaAccountUserType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCases]" caption="PaymentUseCases" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCases].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCases].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessChannel].[DimProcessChannelID]" caption="DimProcessChannelID" attribute="1" defaultMemberUniqueName="[ProcessChannel].[DimProcessChannelID].[All]" allUniqueName="[ProcessChannel].[DimProcessChannelID].[All]" dimensionUniqueName="[ProcessChannel]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessChannel].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[ProcessChannel].[Name].[All]" allUniqueName="[ProcessChannel].[Name].[All]" dimensionUniqueName="[ProcessChannel]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessChannel].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[ProcessChannel].[SourceKey].[All]" allUniqueName="[ProcessChannel].[SourceKey].[All]" dimensionUniqueName="[ProcessChannel]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessChannel].[TextDesciption]" caption="TextDesciption" attribute="1" defaultMemberUniqueName="[ProcessChannel].[TextDesciption].[All]" allUniqueName="[ProcessChannel].[TextDesciption].[All]" dimensionUniqueName="[ProcessChannel]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[Date]" caption="Date" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[ProcessCompletedDate].[Date].[All]" allUniqueName="[ProcessCompletedDate].[Date].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" memberValueDatatype="7" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[DateID]" caption="DateID" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[DateID].[All]" allUniqueName="[ProcessCompletedDate].[DateID].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[DateSK]" caption="DateSK" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[DateSK].[All]" allUniqueName="[ProcessCompletedDate].[DateSK].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[Day]" caption="Day" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[Day].[All]" allUniqueName="[ProcessCompletedDate].[Day].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[DayOfWeek].[All]" allUniqueName="[ProcessCompletedDate].[DayOfWeek].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[DayOfYear]" caption="DayOfYear" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[DayOfYear].[All]" allUniqueName="[ProcessCompletedDate].[DayOfYear].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[DaySuffix]" caption="DaySuffix" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[DaySuffix].[All]" allUniqueName="[ProcessCompletedDate].[DaySuffix].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[DOWInMonth].[All]" allUniqueName="[ProcessCompletedDate].[DOWInMonth].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[FinancialPeriodAllTime].[All]" allUniqueName="[ProcessCompletedDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[FinancialPeriodName].[All]" allUniqueName="[ProcessCompletedDate].[FinancialPeriodName].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[FinancialPeriodNumber].[All]" allUniqueName="[ProcessCompletedDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[FinancialYearName].[All]" allUniqueName="[ProcessCompletedDate].[FinancialYearName].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[FinancialYearNumber].[All]" allUniqueName="[ProcessCompletedDate].[FinancialYearNumber].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[HolidayText]" caption="HolidayText" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[HolidayText].[All]" allUniqueName="[ProcessCompletedDate].[HolidayText].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[IsPublicHoliday].[All]" allUniqueName="[ProcessCompletedDate].[IsPublicHoliday].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[MonthAllTime].[All]" allUniqueName="[ProcessCompletedDate].[MonthAllTime].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[MonthName]" caption="MonthName" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[MonthName].[All]" allUniqueName="[ProcessCompletedDate].[MonthName].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[MonthNumber]" caption="MonthNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[MonthNumber].[All]" allUniqueName="[ProcessCompletedDate].[MonthNumber].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[Quarter]" caption="Quarter" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[Quarter].[All]" allUniqueName="[ProcessCompletedDate].[Quarter].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[QuarterAllTime].[All]" allUniqueName="[ProcessCompletedDate].[QuarterAllTime].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[QuarterName]" caption="QuarterName" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[QuarterName].[All]" allUniqueName="[ProcessCompletedDate].[QuarterName].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[StandardDate]" caption="StandardDate" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[StandardDate].[All]" allUniqueName="[ProcessCompletedDate].[StandardDate].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[USDayOfWeek].[All]" allUniqueName="[ProcessCompletedDate].[USDayOfWeek].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[WeekOfMonth].[All]" allUniqueName="[ProcessCompletedDate].[WeekOfMonth].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[WeekOfYear].[All]" allUniqueName="[ProcessCompletedDate].[WeekOfYear].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[YearName]" caption="YearName" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[YearName].[All]" allUniqueName="[ProcessCompletedDate].[YearName].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessCompletedDate].[YearNumber]" caption="YearNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessCompletedDate].[YearNumber].[All]" allUniqueName="[ProcessCompletedDate].[YearNumber].[All]" dimensionUniqueName="[ProcessCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[AgentCommissionAmount]" caption="AgentCommissionAmount" attribute="1" defaultMemberUniqueName="[ProcessEvent].[AgentCommissionAmount].[All]" allUniqueName="[ProcessEvent].[AgentCommissionAmount].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[ATMReferenceNumber]" caption="ATMReferenceNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[ATMReferenceNumber].[All]" allUniqueName="[ProcessEvent].[ATMReferenceNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[CardProcessorName]" caption="CardProcessorName" attribute="1" defaultMemberUniqueName="[ProcessEvent].[CardProcessorName].[All]" allUniqueName="[ProcessEvent].[CardProcessorName].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[CustomerBillerAccount]" caption="CustomerBillerAccount" attribute="1" defaultMemberUniqueName="[ProcessEvent].[CustomerBillerAccount].[All]" allUniqueName="[ProcessEvent].[CustomerBillerAccount].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[CustomerPhoneNumber]" caption="CustomerPhoneNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[CustomerPhoneNumber].[All]" allUniqueName="[ProcessEvent].[CustomerPhoneNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DepositNumber]" caption="DepositNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DepositNumber].[All]" allUniqueName="[ProcessEvent].[DepositNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimAgentCommissionTypeID]" caption="DimAgentCommissionTypeID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimAgentCommissionTypeID].[All]" allUniqueName="[ProcessEvent].[DimAgentCommissionTypeID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimApprovedByUserID]" caption="DimApprovedByUserID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimApprovedByUserID].[All]" allUniqueName="[ProcessEvent].[DimApprovedByUserID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimCancellationApprovedByUserID]" caption="DimCancellationApprovedByUserID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimCancellationApprovedByUserID].[All]" allUniqueName="[ProcessEvent].[DimCancellationApprovedByUserID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimCompletedDateID]" caption="DimCompletedDateID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimCompletedDateID].[All]" allUniqueName="[ProcessEvent].[DimCompletedDateID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimCompletedTimeID]" caption="DimCompletedTimeID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimCompletedTimeID].[All]" allUniqueName="[ProcessEvent].[DimCompletedTimeID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimForUserID]" caption="DimForUserID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimForUserID].[All]" allUniqueName="[ProcessEvent].[DimForUserID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimInitiatingUserID]" caption="DimInitiatingUserID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimInitiatingUserID].[All]" allUniqueName="[ProcessEvent].[DimInitiatingUserID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimProcessChannelID]" caption="DimProcessChannelID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimProcessChannelID].[All]" allUniqueName="[ProcessEvent].[DimProcessChannelID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimProcessStatusID]" caption="DimProcessStatusID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimProcessStatusID].[All]" allUniqueName="[ProcessEvent].[DimProcessStatusID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimProcessTypeID]" caption="DimProcessTypeID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimProcessTypeID].[All]" allUniqueName="[ProcessEvent].[DimProcessTypeID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimRequestedProcessChannelID]" caption="DimRequestedProcessChannelID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimRequestedProcessChannelID].[All]" allUniqueName="[ProcessEvent].[DimRequestedProcessChannelID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimStartedDateID]" caption="DimStartedDateID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimStartedDateID].[All]" allUniqueName="[ProcessEvent].[DimStartedDateID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimStartedTimeID]" caption="DimStartedTimeID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimStartedTimeID].[All]" allUniqueName="[ProcessEvent].[DimStartedTimeID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimToUserID]" caption="DimToUserID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimToUserID].[All]" allUniqueName="[ProcessEvent].[DimToUserID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimUserID]" caption="DimUserID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimUserID].[All]" allUniqueName="[ProcessEvent].[DimUserID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[DimVerifiedByUserID]" caption="DimVerifiedByUserID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[DimVerifiedByUserID].[All]" allUniqueName="[ProcessEvent].[DimVerifiedByUserID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[FactDependentProcessEventID]" caption="FactDependentProcessEventID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[FactDependentProcessEventID].[All]" allUniqueName="[ProcessEvent].[FactDependentProcessEventID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[FactOriginalProcessEventID]" caption="FactOriginalProcessEventID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[FactOriginalProcessEventID].[All]" allUniqueName="[ProcessEvent].[FactOriginalProcessEventID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[FactProcessEventID]" caption="FactProcessEventID" attribute="1" defaultMemberUniqueName="[ProcessEvent].[FactProcessEventID].[All]" allUniqueName="[ProcessEvent].[FactProcessEventID].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[HasFinancialTransaction]" caption="HasFinancialTransaction" attribute="1" defaultMemberUniqueName="[ProcessEvent].[HasFinancialTransaction].[All]" allUniqueName="[ProcessEvent].[HasFinancialTransaction].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[IntegrationReferenceNumber]" caption="IntegrationReferenceNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[IntegrationReferenceNumber].[All]" allUniqueName="[ProcessEvent].[IntegrationReferenceNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[LinkedPhoneNumber]" caption="LinkedPhoneNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[LinkedPhoneNumber].[All]" allUniqueName="[ProcessEvent].[LinkedPhoneNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[MerchantConfirmationCode]" caption="MerchantConfirmationCode" attribute="1" defaultMemberUniqueName="[ProcessEvent].[MerchantConfirmationCode].[All]" allUniqueName="[ProcessEvent].[MerchantConfirmationCode].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[MerchantCustomerAccountNumber]" caption="MerchantCustomerAccountNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[MerchantCustomerAccountNumber].[All]" allUniqueName="[ProcessEvent].[MerchantCustomerAccountNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[PaymentSource]" caption="PaymentSource" attribute="1" defaultMemberUniqueName="[ProcessEvent].[PaymentSource].[All]" allUniqueName="[ProcessEvent].[PaymentSource].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[ProcessCode]" caption="ProcessCode" attribute="1" defaultMemberUniqueName="[ProcessEvent].[ProcessCode].[All]" allUniqueName="[ProcessEvent].[ProcessCode].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[ProcessFee]" caption="ProcessFee" attribute="1" defaultMemberUniqueName="[ProcessEvent].[ProcessFee].[All]" allUniqueName="[ProcessEvent].[ProcessFee].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[ProcessTx_Amount]" caption="ProcessTx_Amount" attribute="1" defaultMemberUniqueName="[ProcessEvent].[ProcessTx_Amount].[All]" allUniqueName="[ProcessEvent].[ProcessTx_Amount].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[ReferenceNumber]" caption="ReferenceNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[ReferenceNumber].[All]" allUniqueName="[ProcessEvent].[ReferenceNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[SenderPhoneNumber]" caption="SenderPhoneNumber" attribute="1" defaultMemberUniqueName="[ProcessEvent].[SenderPhoneNumber].[All]" allUniqueName="[ProcessEvent].[SenderPhoneNumber].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[ProcessEvent].[SourceKey].[All]" allUniqueName="[ProcessEvent].[SourceKey].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[VerificationStatus]" caption="VerificationStatus" attribute="1" defaultMemberUniqueName="[ProcessEvent].[VerificationStatus].[All]" allUniqueName="[ProcessEvent].[VerificationStatus].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessEvent].[WithdrawalCode]" caption="WithdrawalCode" attribute="1" defaultMemberUniqueName="[ProcessEvent].[WithdrawalCode].[All]" allUniqueName="[ProcessEvent].[WithdrawalCode].[All]" dimensionUniqueName="[ProcessEvent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[Date]" caption="Date" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[ProcessStartedDate].[Date].[All]" allUniqueName="[ProcessStartedDate].[Date].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" memberValueDatatype="7" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[DateID]" caption="DateID" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[DateID].[All]" allUniqueName="[ProcessStartedDate].[DateID].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[DateSK]" caption="DateSK" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[DateSK].[All]" allUniqueName="[ProcessStartedDate].[DateSK].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[Day]" caption="Day" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[Day].[All]" allUniqueName="[ProcessStartedDate].[Day].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[DayOfWeek].[All]" allUniqueName="[ProcessStartedDate].[DayOfWeek].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[DayOfYear]" caption="DayOfYear" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[DayOfYear].[All]" allUniqueName="[ProcessStartedDate].[DayOfYear].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[DaySuffix]" caption="DaySuffix" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[DaySuffix].[All]" allUniqueName="[ProcessStartedDate].[DaySuffix].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[DOWInMonth].[All]" allUniqueName="[ProcessStartedDate].[DOWInMonth].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[FinancialPeriodAllTime].[All]" allUniqueName="[ProcessStartedDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[FinancialPeriodName].[All]" allUniqueName="[ProcessStartedDate].[FinancialPeriodName].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[FinancialPeriodNumber].[All]" allUniqueName="[ProcessStartedDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[FinancialYearName].[All]" allUniqueName="[ProcessStartedDate].[FinancialYearName].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[FinancialYearNumber].[All]" allUniqueName="[ProcessStartedDate].[FinancialYearNumber].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[HolidayText]" caption="HolidayText" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[HolidayText].[All]" allUniqueName="[ProcessStartedDate].[HolidayText].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[IsPublicHoliday].[All]" allUniqueName="[ProcessStartedDate].[IsPublicHoliday].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[MonthAllTime].[All]" allUniqueName="[ProcessStartedDate].[MonthAllTime].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[MonthName]" caption="MonthName" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[MonthName].[All]" allUniqueName="[ProcessStartedDate].[MonthName].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[MonthNumber]" caption="MonthNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[MonthNumber].[All]" allUniqueName="[ProcessStartedDate].[MonthNumber].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[Quarter]" caption="Quarter" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[Quarter].[All]" allUniqueName="[ProcessStartedDate].[Quarter].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[QuarterAllTime].[All]" allUniqueName="[ProcessStartedDate].[QuarterAllTime].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[QuarterName]" caption="QuarterName" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[QuarterName].[All]" allUniqueName="[ProcessStartedDate].[QuarterName].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[StandardDate]" caption="StandardDate" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[StandardDate].[All]" allUniqueName="[ProcessStartedDate].[StandardDate].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[USDayOfWeek].[All]" allUniqueName="[ProcessStartedDate].[USDayOfWeek].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[WeekOfMonth].[All]" allUniqueName="[ProcessStartedDate].[WeekOfMonth].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[WeekOfYear].[All]" allUniqueName="[ProcessStartedDate].[WeekOfYear].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[YearName]" caption="YearName" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[YearName].[All]" allUniqueName="[ProcessStartedDate].[YearName].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStartedDate].[YearNumber]" caption="YearNumber" attribute="1" time="1" defaultMemberUniqueName="[ProcessStartedDate].[YearNumber].[All]" allUniqueName="[ProcessStartedDate].[YearNumber].[All]" dimensionUniqueName="[ProcessStartedDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStatus].[DimProcessStatusID]" caption="DimProcessStatusID" attribute="1" defaultMemberUniqueName="[ProcessStatus].[DimProcessStatusID].[All]" allUniqueName="[ProcessStatus].[DimProcessStatusID].[All]" dimensionUniqueName="[ProcessStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStatus].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[ProcessStatus].[Name].[All]" allUniqueName="[ProcessStatus].[Name].[All]" dimensionUniqueName="[ProcessStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessStatus].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[ProcessStatus].[SourceKey].[All]" allUniqueName="[ProcessStatus].[SourceKey].[All]" dimensionUniqueName="[ProcessStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessType].[DescriptionText]" caption="DescriptionText" attribute="1" defaultMemberUniqueName="[ProcessType].[DescriptionText].[All]" allUniqueName="[ProcessType].[DescriptionText].[All]" dimensionUniqueName="[ProcessType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessType].[DimProcessTypeID]" caption="DimProcessTypeID" attribute="1" defaultMemberUniqueName="[ProcessType].[DimProcessTypeID].[All]" allUniqueName="[ProcessType].[DimProcessTypeID].[All]" dimensionUniqueName="[ProcessType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[ProcessType].[Name].[All]" allUniqueName="[ProcessType].[Name].[All]" dimensionUniqueName="[ProcessType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ProcessType].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[ProcessType].[SourceKey].[All]" allUniqueName="[ProcessType].[SourceKey].[All]" dimensionUniqueName="[ProcessType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[ToUser].[DimCreatedDateID].[All]" allUniqueName="[ToUser].[DimCreatedDateID].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[ToUser].[DimDateOfBirthID].[All]" allUniqueName="[ToUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[DimToUserID]" caption="DimToUserID" attribute="1" defaultMemberUniqueName="[ToUser].[DimToUserID].[All]" allUniqueName="[ToUser].[DimToUserID].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[FirstName]" caption="FirstName" attribute="1" defaultMemberUniqueName="[ToUser].[FirstName].[All]" allUniqueName="[ToUser].[FirstName].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[ToUser].[Gender].[All]" allUniqueName="[ToUser].[Gender].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[IsEnabled]" caption="IsEnabled" attribute="1" defaultMemberUniqueName="[ToUser].[IsEnabled].[All]" allUniqueName="[ToUser].[IsEnabled].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[LastName]" caption="LastName" attribute="1" defaultMemberUniqueName="[ToUser].[LastName].[All]" allUniqueName="[ToUser].[LastName].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[MiddleName]" caption="MiddleName" attribute="1" defaultMemberUniqueName="[ToUser].[MiddleName].[All]" allUniqueName="[ToUser].[MiddleName].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[ToUser].[Name].[All]" allUniqueName="[ToUser].[Name].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[RoleName]" caption="RoleName" attribute="1" defaultMemberUniqueName="[ToUser].[RoleName].[All]" allUniqueName="[ToUser].[RoleName].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[ToUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[ToUser].[SourceKey].[All]" allUniqueName="[ToUser].[SourceKey].[All]" dimensionUniqueName="[ToUser]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[Date]" caption="Date" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[TransactionDate].[Date].[All]" allUniqueName="[TransactionDate].[Date].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" memberValueDatatype="7" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[DateID]" caption="DateID" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[DateID].[All]" allUniqueName="[TransactionDate].[DateID].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[DateSK]" caption="DateSK" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[DateSK].[All]" allUniqueName="[TransactionDate].[DateSK].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[Day]" caption="Day" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[Day].[All]" allUniqueName="[TransactionDate].[Day].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[DayOfWeek].[All]" allUniqueName="[TransactionDate].[DayOfWeek].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[DayOfYear]" caption="DayOfYear" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[DayOfYear].[All]" allUniqueName="[TransactionDate].[DayOfYear].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[DaySuffix]" caption="DaySuffix" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[DaySuffix].[All]" allUniqueName="[TransactionDate].[DaySuffix].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[DOWInMonth].[All]" allUniqueName="[TransactionDate].[DOWInMonth].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[FinancialPeriodAllTime].[All]" allUniqueName="[TransactionDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[FinancialPeriodName].[All]" allUniqueName="[TransactionDate].[FinancialPeriodName].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[FinancialPeriodNumber].[All]" allUniqueName="[TransactionDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[FinancialYearName].[All]" allUniqueName="[TransactionDate].[FinancialYearName].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[FinancialYearNumber].[All]" allUniqueName="[TransactionDate].[FinancialYearNumber].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[HolidayText]" caption="HolidayText" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[HolidayText].[All]" allUniqueName="[TransactionDate].[HolidayText].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[IsPublicHoliday].[All]" allUniqueName="[TransactionDate].[IsPublicHoliday].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[MonthAllTime].[All]" allUniqueName="[TransactionDate].[MonthAllTime].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[MonthName]" caption="MonthName" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[MonthName].[All]" allUniqueName="[TransactionDate].[MonthName].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[MonthNumber]" caption="MonthNumber" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[MonthNumber].[All]" allUniqueName="[TransactionDate].[MonthNumber].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[Quarter]" caption="Quarter" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[Quarter].[All]" allUniqueName="[TransactionDate].[Quarter].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[QuarterAllTime].[All]" allUniqueName="[TransactionDate].[QuarterAllTime].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[QuarterName]" caption="QuarterName" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[QuarterName].[All]" allUniqueName="[TransactionDate].[QuarterName].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[StandardDate]" caption="StandardDate" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[StandardDate].[All]" allUniqueName="[TransactionDate].[StandardDate].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[USDayOfWeek].[All]" allUniqueName="[TransactionDate].[USDayOfWeek].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[WeekOfMonth].[All]" allUniqueName="[TransactionDate].[WeekOfMonth].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[WeekOfYear].[All]" allUniqueName="[TransactionDate].[WeekOfYear].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[YearName]" caption="YearName" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[YearName].[All]" allUniqueName="[TransactionDate].[YearName].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TransactionDate].[YearNumber]" caption="YearNumber" attribute="1" time="1" defaultMemberUniqueName="[TransactionDate].[YearNumber].[All]" allUniqueName="[TransactionDate].[YearNumber].[All]" dimensionUniqueName="[TransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[User].[DimCreatedDateID].[All]" allUniqueName="[User].[DimCreatedDateID].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[User].[DimDateOfBirthID].[All]" allUniqueName="[User].[DimDateOfBirthID].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[DimUserID]" caption="DimUserID" attribute="1" defaultMemberUniqueName="[User].[DimUserID].[All]" allUniqueName="[User].[DimUserID].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[FirstName]" caption="FirstName" attribute="1" defaultMemberUniqueName="[User].[FirstName].[All]" allUniqueName="[User].[FirstName].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[User].[Gender].[All]" allUniqueName="[User].[Gender].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[IsEnabled]" caption="IsEnabled" attribute="1" defaultMemberUniqueName="[User].[IsEnabled].[All]" allUniqueName="[User].[IsEnabled].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[LastName]" caption="LastName" attribute="1" defaultMemberUniqueName="[User].[LastName].[All]" allUniqueName="[User].[LastName].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[MiddleName]" caption="MiddleName" attribute="1" defaultMemberUniqueName="[User].[MiddleName].[All]" allUniqueName="[User].[MiddleName].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[User].[Name].[All]" allUniqueName="[User].[Name].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[RoleName]" caption="RoleName" attribute="1" defaultMemberUniqueName="[User].[RoleName].[All]" allUniqueName="[User].[RoleName].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[User].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[User].[SourceKey].[All]" allUniqueName="[User].[SourceKey].[All]" dimensionUniqueName="[User]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[DimBankAccountID]" caption="DimBankAccountID" attribute="1" defaultMemberUniqueName="[FinancialAccount].[DimBankAccountID].[All]" allUniqueName="[FinancialAccount].[DimBankAccountID].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[DimCurrencyID]" caption="DimCurrencyID" attribute="1" defaultMemberUniqueName="[FinancialAccount].[DimCurrencyID].[All]" allUniqueName="[FinancialAccount].[DimCurrencyID].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[DimFinancialHoldingAccountID]" caption="DimFinancialHoldingAccountID" attribute="1" defaultMemberUniqueName="[FinancialAccount].[DimFinancialHoldingAccountID].[All]" allUniqueName="[FinancialAccount].[DimFinancialHoldingAccountID].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[FinancialAccount].[DimPagaAccountID].[All]" allUniqueName="[FinancialAccount].[DimPagaAccountID].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialTransactionType].[DimFinancialTxTypeID]" caption="DimFinancialTxTypeID" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" allUniqueName="[FinancialTransactionType].[DimFinancialTxTypeID].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTxCategory]" caption="FinancialTxCategory" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" allUniqueName="[FinancialTransactionType].[FinancialTxCategory].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[FinancialTransactionType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[Name].[All]" allUniqueName="[FinancialTransactionType].[Name].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[DimGLCodeID]" caption="DimGLCodeID" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[DimGLCodeID].[All]" allUniqueName="[GLCodeHierarchy].[DimGLCodeID].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[GLCode]" caption="GLCode" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[GLCode].[All]" allUniqueName="[GLCodeHierarchy].[GLCode].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[MainHeading]" caption="MainHeading" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[MainHeading].[All]" allUniqueName="[GLCodeHierarchy].[MainHeading].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[SubHeading_1]" caption="SubHeading_1" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[SubHeading_1].[All]" allUniqueName="[GLCodeHierarchy].[SubHeading_1].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[SubHeading_2]" caption="SubHeading_2" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[SubHeading_2].[All]" allUniqueName="[GLCodeHierarchy].[SubHeading_2].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[SubHeading_3]" caption="SubHeading_3" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[SubHeading_3].[All]" allUniqueName="[GLCodeHierarchy].[SubHeading_3].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLCodeHierarchy].[SubHeading_4]" caption="SubHeading_4" attribute="1" defaultMemberUniqueName="[GLCodeHierarchy].[SubHeading_4].[All]" allUniqueName="[GLCodeHierarchy].[SubHeading_4].[All]" dimensionUniqueName="[GLCodeHierarchy]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[GLTransaction].[Bal]" caption="Bal" attribute="1" defaultMemberUniqueName="[GLTransaction].[Bal].[All]" allUniqueName="[GLTransaction].[Bal].[All]" dimensionUniqueName="[GLTransaction]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[PaymentUseCase].[DimFinancialTxTypeID]" caption="DimFinancialTxTypeID" attribute="1" defaultMemberUniqueName="[PaymentUseCase].[DimFinancialTxTypeID].[All]" allUniqueName="[PaymentUseCase].[DimFinancialTxTypeID].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCase]" caption="PaymentUseCase" attribute="1" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCase].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCase].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCaseType]" caption="PaymentUseCaseType" attribute="1" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCaseType].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCaseType].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[TxCount]" caption="TxCount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Credits]" caption="Credits" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Debits]" caption="Debits" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Balance]" caption="Balance" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[ProcessEventCount]" caption="ProcessEventCount" measure="1" displayFolder="" measureGroup="ProcessEvent" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[BaseTransaction]" caption="BaseTransaction" measure="1" displayFolder="" measureGroup="FinancialTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[TxAmount]" caption="TxAmount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[ProcessTxAmt]" caption="ProcessTxAmt" measure="1" displayFolder="" measureGroup="ProcessEvent" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransactionType]" caption="_Count FinancialTransactionType" measure="1" displayFolder="" measureGroup="FinancialTransactionType" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count FinancialAccount]" caption="_Count FinancialAccount" measure="1" displayFolder="" measureGroup="FinancialAccount" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count FinancialTransaction]" caption="_Count FinancialTransaction" measure="1" displayFolder="" measureGroup="FinancialTransaction" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count GLTransaction]" caption="_Count GLTransaction" measure="1" displayFolder="" measureGroup="GLTransaction" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count TransactionDate]" caption="_Count TransactionDate" measure="1" displayFolder="" measureGroup="TransactionDate" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count GLCodeHierarchy]" caption="_Count GLCodeHierarchy" measure="1" displayFolder="" measureGroup="GLCodeHierarchy" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ForUser]" caption="_Count ForUser" measure="1" displayFolder="" measureGroup="ForUser" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count InitiatingUser]" caption="_Count InitiatingUser" measure="1" displayFolder="" measureGroup="InitiatingUser" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ToUser]" caption="_Count ToUser" measure="1" displayFolder="" measureGroup="ToUser" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count User]" caption="_Count User" measure="1" displayFolder="" measureGroup="User" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ProcessEvent]" caption="_Count ProcessEvent" measure="1" displayFolder="" measureGroup="ProcessEvent" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count Organization]" caption="_Count Organization" measure="1" displayFolder="" measureGroup="Organization" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count PagaAccount]" caption="_Count PagaAccount" measure="1" displayFolder="" measureGroup="PagaAccount" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count BankingStatus]" caption="_Count BankingStatus" measure="1" displayFolder="" measureGroup="BankingStatus" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count PagaAccountStatus]" caption="_Count PagaAccountStatus" measure="1" displayFolder="" measureGroup="PagaAccountStatus" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count PagaAccountUserType]" caption="_Count PagaAccountUserType" measure="1" displayFolder="" measureGroup="PagaAccountUserType" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ProcessChannel]" caption="_Count ProcessChannel" measure="1" displayFolder="" measureGroup="ProcessChannel" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ProcessStatus]" caption="_Count ProcessStatus" measure="1" displayFolder="" measureGroup="ProcessStatus" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ProcessType]" caption="_Count ProcessType" measure="1" displayFolder="" measureGroup="ProcessType" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ProcessCompletedDate]" caption="_Count ProcessCompletedDate" measure="1" displayFolder="" measureGroup="ProcessCompletedDate" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count ProcessStartedDate]" caption="_Count ProcessStartedDate" measure="1" displayFolder="" measureGroup="ProcessStartedDate" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count PaymentUseCase]" caption="_Count PaymentUseCase" measure="1" displayFolder="" measureGroup="PaymentUseCase" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count LatestFinancialTransaction]" caption="_Count LatestFinancialTransaction" measure="1" displayFolder="" measureGroup="LatestFinancialTransaction" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="24">
+    <dimension name="BankingStatus" uniqueName="[BankingStatus]" caption="BankingStatus"/>
+    <dimension name="FinancialAccount" uniqueName="[FinancialAccount]" caption="FinancialAccount"/>
+    <dimension name="FinancialTransaction" uniqueName="[FinancialTransaction]" caption="FinancialTransaction"/>
+    <dimension name="FinancialTransactionType" uniqueName="[FinancialTransactionType]" caption="FinancialTransactionType"/>
+    <dimension name="ForUser" uniqueName="[ForUser]" caption="ForUser"/>
+    <dimension name="GLCodeHierarchy" uniqueName="[GLCodeHierarchy]" caption="GLCodeHierarchy"/>
+    <dimension name="GLTransaction" uniqueName="[GLTransaction]" caption="GLTransaction"/>
+    <dimension name="InitiatingUser" uniqueName="[InitiatingUser]" caption="InitiatingUser"/>
+    <dimension name="LatestFinancialTransaction" uniqueName="[LatestFinancialTransaction]" caption="LatestFinancialTransaction"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Organization" uniqueName="[Organization]" caption="Organization"/>
+    <dimension name="PagaAccount" uniqueName="[PagaAccount]" caption="PagaAccount"/>
+    <dimension name="PagaAccountStatus" uniqueName="[PagaAccountStatus]" caption="PagaAccountStatus"/>
+    <dimension name="PagaAccountUserType" uniqueName="[PagaAccountUserType]" caption="PagaAccountUserType"/>
+    <dimension name="PaymentUseCase" uniqueName="[PaymentUseCase]" caption="PaymentUseCase"/>
+    <dimension name="ProcessChannel" uniqueName="[ProcessChannel]" caption="ProcessChannel"/>
+    <dimension name="ProcessCompletedDate" uniqueName="[ProcessCompletedDate]" caption="ProcessCompletedDate"/>
+    <dimension name="ProcessEvent" uniqueName="[ProcessEvent]" caption="ProcessEvent"/>
+    <dimension name="ProcessStartedDate" uniqueName="[ProcessStartedDate]" caption="ProcessStartedDate"/>
+    <dimension name="ProcessStatus" uniqueName="[ProcessStatus]" caption="ProcessStatus"/>
+    <dimension name="ProcessType" uniqueName="[ProcessType]" caption="ProcessType"/>
+    <dimension name="ToUser" uniqueName="[ToUser]" caption="ToUser"/>
+    <dimension name="TransactionDate" uniqueName="[TransactionDate]" caption="TransactionDate"/>
+    <dimension name="User" uniqueName="[User]" caption="User"/>
+  </dimensions>
+  <measureGroups count="23">
+    <measureGroup name="BankingStatus" caption="BankingStatus"/>
+    <measureGroup name="FinancialAccount" caption="FinancialAccount"/>
+    <measureGroup name="FinancialTransaction" caption="FinancialTransaction"/>
+    <measureGroup name="FinancialTransactionType" caption="FinancialTransactionType"/>
+    <measureGroup name="ForUser" caption="ForUser"/>
+    <measureGroup name="GLCodeHierarchy" caption="GLCodeHierarchy"/>
+    <measureGroup name="GLTransaction" caption="GLTransaction"/>
+    <measureGroup name="InitiatingUser" caption="InitiatingUser"/>
+    <measureGroup name="LatestFinancialTransaction" caption="LatestFinancialTransaction"/>
+    <measureGroup name="Organization" caption="Organization"/>
+    <measureGroup name="PagaAccount" caption="PagaAccount"/>
+    <measureGroup name="PagaAccountStatus" caption="PagaAccountStatus"/>
+    <measureGroup name="PagaAccountUserType" caption="PagaAccountUserType"/>
+    <measureGroup name="PaymentUseCase" caption="PaymentUseCase"/>
+    <measureGroup name="ProcessChannel" caption="ProcessChannel"/>
+    <measureGroup name="ProcessCompletedDate" caption="ProcessCompletedDate"/>
+    <measureGroup name="ProcessEvent" caption="ProcessEvent"/>
+    <measureGroup name="ProcessStartedDate" caption="ProcessStartedDate"/>
+    <measureGroup name="ProcessStatus" caption="ProcessStatus"/>
+    <measureGroup name="ProcessType" caption="ProcessType"/>
+    <measureGroup name="ToUser" caption="ToUser"/>
+    <measureGroup name="TransactionDate" caption="TransactionDate"/>
+    <measureGroup name="User" caption="User"/>
+  </measureGroups>
+  <maps count="61">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="1" dimension="1"/>
+    <map measureGroup="2" dimension="2"/>
+    <map measureGroup="2" dimension="3"/>
+    <map measureGroup="2" dimension="4"/>
+    <map measureGroup="2" dimension="7"/>
+    <map measureGroup="2" dimension="15"/>
+    <map measureGroup="2" dimension="16"/>
+    <map measureGroup="2" dimension="17"/>
+    <map measureGroup="2" dimension="18"/>
+    <map measureGroup="2" dimension="19"/>
+    <map measureGroup="2" dimension="20"/>
+    <map measureGroup="2" dimension="21"/>
+    <map measureGroup="2" dimension="22"/>
+    <map measureGroup="2" dimension="23"/>
+    <map measureGroup="3" dimension="3"/>
+    <map measureGroup="4" dimension="4"/>
+    <map measureGroup="5" dimension="5"/>
+    <map measureGroup="6" dimension="1"/>
+    <map measureGroup="6" dimension="2"/>
+    <map measureGroup="6" dimension="3"/>
+    <map measureGroup="6" dimension="4"/>
+    <map measureGroup="6" dimension="5"/>
+    <map measureGroup="6" dimension="6"/>
+    <map measureGroup="6" dimension="7"/>
+    <map measureGroup="6" dimension="15"/>
+    <map measureGroup="6" dimension="16"/>
+    <map measureGroup="6" dimension="17"/>
+    <map measureGroup="6" dimension="18"/>
+    <map measureGroup="6" dimension="19"/>
+    <map measureGroup="6" dimension="20"/>
+    <map measureGroup="6" dimension="21"/>
+    <map measureGroup="6" dimension="22"/>
+    <map measureGroup="6" dimension="23"/>
+    <map measureGroup="7" dimension="7"/>
+    <map measureGroup="8" dimension="8"/>
+    <map measureGroup="9" dimension="10"/>
+    <map measureGroup="10" dimension="11"/>
+    <map measureGroup="10" dimension="12"/>
+    <map measureGroup="11" dimension="12"/>
+    <map measureGroup="12" dimension="13"/>
+    <map measureGroup="13" dimension="3"/>
+    <map measureGroup="13" dimension="14"/>
+    <map measureGroup="14" dimension="15"/>
+    <map measureGroup="15" dimension="16"/>
+    <map measureGroup="16" dimension="4"/>
+    <map measureGroup="16" dimension="7"/>
+    <map measureGroup="16" dimension="15"/>
+    <map measureGroup="16" dimension="16"/>
+    <map measureGroup="16" dimension="17"/>
+    <map measureGroup="16" dimension="18"/>
+    <map measureGroup="16" dimension="19"/>
+    <map measureGroup="16" dimension="20"/>
+    <map measureGroup="16" dimension="21"/>
+    <map measureGroup="16" dimension="23"/>
+    <map measureGroup="17" dimension="18"/>
+    <map measureGroup="18" dimension="19"/>
+    <map measureGroup="19" dimension="20"/>
+    <map measureGroup="20" dimension="21"/>
+    <map measureGroup="21" dimension="22"/>
+    <map measureGroup="22" dimension="23"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42067.657969328706" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="9">
+    <cacheField name="[Measures].[Debits]" caption="Debits" numFmtId="0" hierarchy="291" level="32767"/>
+    <cacheField name="[Measures].[Credits]" caption="Credits" numFmtId="0" hierarchy="290" level="32767"/>
+    <cacheField name="[Measures].[Balance]" caption="Balance" numFmtId="0" hierarchy="292" level="32767"/>
+    <cacheField name="[GLCodeHierarchy].[GLCodes].[MainHeading]" caption="MainHeading" numFmtId="0" hierarchy="46" level="1">
+      <sharedItems count="2">
+        <s v="[GLCodeHierarchy].[GLCodes].[MainHeading].&amp;[Chart of Accounts]" c="Chart of Accounts"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[MainHeading].&amp;" c=""/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_1]" caption="SubHeading_1" numFmtId="0" hierarchy="46" level="2">
+      <sharedItems count="3">
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_1].&amp;[Assets]" c="Assets"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_1].&amp;[Liabilities]" c="Liabilities"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_1].&amp;" c=""/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_2]" caption="SubHeading_2" numFmtId="0" hierarchy="46" level="3">
+      <sharedItems count="4">
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;[10100 - 19999:  Other Assets]" c="10100 - 19999:  Other Assets"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;[12000 - 12999:  Receivables]" c="12000 - 12999:  Receivables"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;[20000 - 29999:  Liabilities]" c="20000 - 29999:  Liabilities"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_2].&amp;" c=""/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_3]" caption="SubHeading_3" numFmtId="0" hierarchy="46" level="4">
+      <sharedItems count="5">
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[12100 - 12399:  Paga Receivables]" c="12100 - 12399:  Paga Receivables"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[12400 - 12499:  Other Receivables]" c="12400 - 12499:  Other Receivables"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[21000 - 21299:  Creditor Others]" c="21000 - 21299:  Creditor Others"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;[22000 - 22999:  Creditors - Pagatech Income]" c="22000 - 22999:  Creditors - Pagatech Income"/>
+        <s v="[GLCodeHierarchy].[GLCodes].[SubHeading_3].&amp;" c=""/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[GLCodeHierarchy].[GLCodes].[SubHeading_4]" caption="SubHeading_4" numFmtId="0" hierarchy="46" level="5">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[TransactionDate].[Date].[Date]" caption="Date" numFmtId="0" hierarchy="233" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="321">
+    <cacheHierarchy uniqueName="[BankingStatus].[BankingStatus]" caption="BankingStatus" attribute="1" defaultMemberUniqueName="[BankingStatus].[BankingStatus].[All]" allUniqueName="[BankingStatus].[BankingStatus].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[BankingStatus].[DimBankingStatusID]" caption="DimBankingStatusID" attribute="1" defaultMemberUniqueName="[BankingStatus].[DimBankingStatusID].[All]" allUniqueName="[BankingStatus].[DimBankingStatusID].[All]" dimensionUniqueName="[BankingStatus]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[AccountNumber]" caption="AccountNumber" attribute="1" defaultMemberUniqueName="[FinancialAccount].[AccountNumber].[All]" allUniqueName="[FinancialAccount].[AccountNumber].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[DimFinancialAccountID]" caption="DimFinancialAccountID" attribute="1" defaultMemberUniqueName="[FinancialAccount].[DimFinancialAccountID].[All]" allUniqueName="[FinancialAccount].[DimFinancialAccountID].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[FinancialAccountID]" caption="FinancialAccountID" attribute="1" defaultMemberUniqueName="[FinancialAccount].[FinancialAccountID].[All]" allUniqueName="[FinancialAccount].[FinancialAccountID].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[FinancialAccountType]" caption="FinancialAccountType" attribute="1" defaultMemberUniqueName="[FinancialAccount].[FinancialAccountType].[All]" allUniqueName="[FinancialAccount].[FinancialAccountType].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[FinancialAccount].[Name].[All]" allUniqueName="[FinancialAccount].[Name].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[OpeningBalance]" caption="OpeningBalance" attribute="1" defaultMemberUniqueName="[FinancialAccount].[OpeningBalance].[All]" allUniqueName="[FinancialAccount].[OpeningBalance].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[FinancialAccount].[RestrictedBalance].[All]" allUniqueName="[FinancialAccount].[RestrictedBalance].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialAccount].[TotalBalance]" caption="TotalBalance" attribute="1" defaultMemberUniqueName="[FinancialAccount].[TotalBalance].[All]" allUniqueName="[FinancialAccount].[TotalBalance].[All]" dimensionUniqueName="[FinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransaction].[Cancelled]" caption="Cancelled" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[Cancelled].[All]" allUniqueName="[FinancialTransaction].[Cancelled].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="2" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[DimCurrencyID]" caption="DimCurrencyID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimCurrencyID].[All]" allUniqueName="[FinancialTransaction].[DimCurrencyID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[DimEffectiveDateID]" caption="DimEffectiveDateID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimEffectiveDateID].[All]" allUniqueName="[FinancialTransaction].[DimEffectiveDateID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[DimEffectiveTimeID]" caption="DimEffectiveTimeID" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[DimEffectiveTimeID].[All]" allUniqueName="[FinancialTransaction].[DimEffectiveTimeID].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
@@ -513,12 +904,7 @@
     <cacheHierarchy uniqueName="[InitiatingUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[InitiatingUser].[SourceKey].[All]" allUniqueName="[InitiatingUser].[SourceKey].[All]" dimensionUniqueName="[InitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[LatestFinancialTransaction].[FactFinancialTxID]" caption="FactFinancialTxID" attribute="1" defaultMemberUniqueName="[LatestFinancialTransaction].[FactFinancialTxID].[All]" allUniqueName="[LatestFinancialTransaction].[FactFinancialTxID].[All]" dimensionUniqueName="[LatestFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[LatestFinancialTransaction].[TransactionDate]" caption="TransactionDate" attribute="1" defaultMemberUniqueName="[LatestFinancialTransaction].[TransactionDate].[All]" allUniqueName="[LatestFinancialTransaction].[TransactionDate].[All]" dimensionUniqueName="[LatestFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[LatestFinancialTransaction].[TransactionTime]" caption="TransactionTime" attribute="1" defaultMemberUniqueName="[LatestFinancialTransaction].[TransactionTime].[All]" allUniqueName="[LatestFinancialTransaction].[TransactionTime].[All]" dimensionUniqueName="[LatestFinancialTransaction]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="9"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[LatestFinancialTransaction].[TransactionTime]" caption="TransactionTime" attribute="1" defaultMemberUniqueName="[LatestFinancialTransaction].[TransactionTime].[All]" allUniqueName="[LatestFinancialTransaction].[TransactionTime].[All]" dimensionUniqueName="[LatestFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Organization].[DimBusinessTypeID]" caption="DimBusinessTypeID" attribute="1" defaultMemberUniqueName="[Organization].[DimBusinessTypeID].[All]" allUniqueName="[Organization].[DimBusinessTypeID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Organization].[DimOrganizationID]" caption="DimOrganizationID" attribute="1" defaultMemberUniqueName="[Organization].[DimOrganizationID].[All]" allUniqueName="[Organization].[DimOrganizationID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Organization].[DimOrganizationSubscriptionStatusID]" caption="DimOrganizationSubscriptionStatusID" attribute="1" defaultMemberUniqueName="[Organization].[DimOrganizationSubscriptionStatusID].[All]" allUniqueName="[Organization].[DimOrganizationSubscriptionStatusID].[All]" dimensionUniqueName="[Organization]" displayFolder="" count="0" unbalanced="0"/>
@@ -909,8 +1295,8 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42062.814683449076" backgroundQuery="1" createdVersion="3" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42067.58467546296" backgroundQuery="1" createdVersion="3" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1">
     <extLst>
       <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
@@ -1245,7 +1631,7 @@
   <kpis count="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition pivotCacheId="11" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+      <x14:pivotCacheDefinition pivotCacheId="16" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{ABF5C744-AB39-4b91-8756-CFA1BBC848D5}">
       <x15:pivotCacheIdVersion cacheIdSupportedVersion="6" cacheIdCreatedVersion="6"/>
@@ -1255,24 +1641,23 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="165" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="5" subtotalHiddenItems="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="General Ledger" colHeaderCaption="Transactions Available Through" fieldListSortAscending="1">
-  <location ref="B21:E61" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="111" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="5" subtotalHiddenItems="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="General Ledger" colHeaderCaption="Transactions Available Through" fieldListSortAscending="1">
+  <location ref="B21:E36" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1">
-      <items count="2">
-        <item c="1" x="0" d="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
       <items count="3">
         <item c="1" x="0" d="1"/>
         <item c="1" x="1" d="1"/>
         <item t="default"/>
       </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
     </pivotField>
     <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
       <items count="4">
@@ -1283,43 +1668,26 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="6">
-        <item c="1" x="0" d="1"/>
+      <items count="5">
+        <item c="1" x="0"/>
         <item c="1" x="1" d="1"/>
         <item c="1" x="2" d="1"/>
         <item c="1" x="3" d="1"/>
-        <item c="1" x="4" d="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="27">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
+      <items count="6">
+        <item c="1" x="0"/>
+        <item c="1" x="1"/>
+        <item c="1" x="2"/>
+        <item c="1" x="3"/>
+        <item c="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
+      <items count="1">
         <item t="default"/>
       </items>
     </pivotField>
@@ -1328,21 +1696,14 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
   </pivotFields>
-  <rowFields count="5">
+  <rowFields count="4">
     <field x="3"/>
     <field x="4"/>
     <field x="5"/>
     <field x="6"/>
-    <field x="7"/>
   </rowFields>
-  <rowItems count="38">
+  <rowItems count="15">
     <i>
       <x/>
     </i>
@@ -1352,47 +1713,14 @@
     <i r="2">
       <x/>
     </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="4">
-      <x/>
-    </i>
-    <i r="4">
-      <x v="1"/>
-    </i>
-    <i r="4">
-      <x v="2"/>
-    </i>
-    <i r="4">
-      <x v="3"/>
-    </i>
-    <i r="4">
-      <x v="4"/>
-    </i>
-    <i r="4">
-      <x v="5"/>
-    </i>
-    <i r="4">
-      <x v="6"/>
-    </i>
-    <i r="4">
-      <x v="7"/>
-    </i>
-    <i r="3">
-      <x v="1"/>
-    </i>
-    <i r="4">
-      <x v="8"/>
-    </i>
     <i r="2">
       <x v="1"/>
     </i>
     <i r="3">
-      <x v="2"/>
+      <x/>
     </i>
-    <i r="4">
-      <x v="9"/>
+    <i r="3">
+      <x v="1"/>
     </i>
     <i r="1">
       <x v="1"/>
@@ -1401,76 +1729,38 @@
       <x v="2"/>
     </i>
     <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="3">
       <x v="3"/>
     </i>
-    <i r="4">
-      <x v="10"/>
+    <i>
+      <x v="1"/>
     </i>
-    <i r="4">
-      <x v="11"/>
+    <i r="1">
+      <x v="2"/>
     </i>
-    <i r="4">
-      <x v="12"/>
-    </i>
-    <i r="4">
-      <x v="13"/>
-    </i>
-    <i r="4">
-      <x v="14"/>
-    </i>
-    <i r="4">
-      <x v="15"/>
-    </i>
-    <i r="4">
-      <x v="16"/>
+    <i r="2">
+      <x v="3"/>
     </i>
     <i r="3">
       <x v="4"/>
-    </i>
-    <i r="4">
-      <x v="17"/>
-    </i>
-    <i r="4">
-      <x v="18"/>
-    </i>
-    <i r="4">
-      <x v="19"/>
-    </i>
-    <i r="4">
-      <x v="20"/>
-    </i>
-    <i r="4">
-      <x v="21"/>
-    </i>
-    <i r="4">
-      <x v="22"/>
-    </i>
-    <i r="4">
-      <x v="23"/>
-    </i>
-    <i r="4">
-      <x v="24"/>
-    </i>
-    <i r="4">
-      <x v="25"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="2">
-    <field x="9"/>
+  <colFields count="1">
     <field x="-2"/>
   </colFields>
   <colItems count="3">
     <i>
       <x/>
-      <x/>
     </i>
-    <i r="1" i="1">
+    <i i="1">
       <x v="1"/>
     </i>
-    <i r="1" i="2">
+    <i i="2">
       <x v="2"/>
     </i>
   </colItems>
@@ -1479,32 +1769,23 @@
     <dataField fld="1" baseField="0" baseItem="0" numFmtId="4"/>
     <dataField fld="2" baseField="0" baseItem="0" numFmtId="4"/>
   </dataFields>
-  <formats count="3">
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+  <formats count="2">
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="9" count="0"/>
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="9" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="2">
             <x v="1"/>
             <x v="2"/>
           </reference>
-          <reference field="9" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
@@ -1834,11 +2115,12 @@
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <filters count="1">
-    <filter fld="8" type="dateEqual" evalOrder="-1" id="4" name="[TransactionDate].[Date]">
+    <filter fld="8" type="dateBetween" evalOrder="-1" id="12" name="[TransactionDate].[Date]">
       <autoFilter ref="A1">
         <filterColumn colId="0">
-          <customFilters>
-            <customFilter val="41281"/>
+          <customFilters and="1">
+            <customFilter operator="greaterThanOrEqual" val="42005"/>
+            <customFilter operator="lessThanOrEqual" val="42035"/>
           </customFilters>
         </filterColumn>
       </autoFilter>
@@ -1852,9 +2134,365 @@
   <rowHierarchiesUsage count="1">
     <rowHierarchyUsage hierarchyUsage="46"/>
   </rowHierarchiesUsage>
-  <colHierarchiesUsage count="2">
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="-2"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="68" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A1:B2" firstHeaderRow="1" firstDataRow="2" firstDataCol="0"/>
+  <pivotFields count="1">
+    <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pivotHierarchies count="321">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <colHierarchiesUsage count="1">
     <colHierarchyUsage hierarchyUsage="71"/>
-    <colHierarchyUsage hierarchyUsage="-2"/>
   </colHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2130,8 +2768,8 @@
   <pivotTables>
     <pivotTable tabId="1" name="PivotTable1"/>
   </pivotTables>
-  <state minimalRefreshVersion="6" lastRefreshVersion="6" pivotCacheId="11" filterType="dateEqual">
-    <selection startDate="2013-01-07T00:00:00" endDate="2013-01-07T00:00:00"/>
+  <state minimalRefreshVersion="6" lastRefreshVersion="6" pivotCacheId="16" filterType="dateBetween">
+    <selection startDate="2015-01-01T00:00:00" endDate="2015-01-31T00:00:00"/>
     <bounds startDate="2010-01-01T00:00:00" endDate="2016-01-01T00:00:00"/>
   </state>
 </timelineCacheDefinition>
@@ -2139,92 +2777,113 @@
 
 <file path=xl/timelines/timeline1.xml><?xml version="1.0" encoding="utf-8"?>
 <timelines xmlns="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <timeline name="Date" cache="Timeline_TransactionDate" caption="TransactionDate" level="3" selectionLevel="3" scrollPosition="2012-12-18T00:00:00"/>
+  <timeline name="Date" cache="Timeline_TransactionDate" caption="TransactionDate" level="2" selectionLevel="2" scrollPosition="2014-05-21T00:00:00"/>
 </timelines>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B21:E61"/>
+  <dimension ref="B10:E36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="78.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="3" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="10" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="str">
+        <f>"Data Available through:  " &amp;Sheet2!A2</f>
+        <v>Data Available through:  3/4/2015 1:30:14 PM</v>
+      </c>
+    </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
-        <v>43</v>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5">
+        <v>10199114012.669981</v>
+      </c>
+      <c r="D22" s="5">
+        <v>10199115012.709984</v>
+      </c>
+      <c r="E22" s="5">
+        <v>-1000.0399814844131</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>26</v>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5">
+        <v>5179701226.3400021</v>
+      </c>
+      <c r="D23" s="5">
+        <v>5108932701.750001</v>
+      </c>
+      <c r="E23" s="5">
+        <v>70768524.590000033</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>40</v>
+      <c r="B24" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C24" s="5">
-        <v>181384414.13000003</v>
+        <v>4990812166.5300016</v>
       </c>
       <c r="D24" s="5">
-        <v>181384414.12</v>
+        <v>4920447970.5600014</v>
       </c>
       <c r="E24" s="5">
-        <v>9.9999941885471344E-3</v>
+        <v>70364195.970000863</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>28</v>
+      <c r="B25" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>136724479.28</v>
+        <v>188889059.80999997</v>
       </c>
       <c r="D25" s="5">
-        <v>119722960.55</v>
+        <v>188484731.18999997</v>
       </c>
       <c r="E25" s="5">
-        <v>17001518.730000004</v>
+        <v>404328.61999998428</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>1</v>
+      <c r="B26" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="C26" s="5">
-        <v>24752666.379999999</v>
+        <v>34885045.069999993</v>
       </c>
       <c r="D26" s="5">
-        <v>24902085</v>
+        <v>30663341.309999999</v>
       </c>
       <c r="E26" s="5">
-        <v>-149418.62</v>
+        <v>4221703.7600000016</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -2232,74 +2891,74 @@
         <v>4</v>
       </c>
       <c r="C27" s="5">
-        <v>2840</v>
+        <v>154004014.73999995</v>
       </c>
       <c r="D27" s="5">
-        <v>0</v>
+        <v>157821389.87999997</v>
       </c>
       <c r="E27" s="5">
-        <v>2840</v>
+        <v>-3817375.1400000136</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>8</v>
+      <c r="B28" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C28" s="5">
-        <v>1810</v>
+        <v>5019412786.3300095</v>
       </c>
       <c r="D28" s="5">
-        <v>0</v>
+        <v>5090182310.9600029</v>
       </c>
       <c r="E28" s="5">
-        <v>1810</v>
+        <v>-70769524.630032808</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>9</v>
+      <c r="B29" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C29" s="5">
-        <v>450</v>
+        <v>5019412786.3300095</v>
       </c>
       <c r="D29" s="5">
-        <v>0</v>
+        <v>5090182310.9600029</v>
       </c>
       <c r="E29" s="5">
-        <v>450</v>
+        <v>-70769524.630032808</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>10</v>
+      <c r="B30" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C30" s="5">
-        <v>280</v>
+        <v>4057473515.3200049</v>
       </c>
       <c r="D30" s="5">
-        <v>0</v>
+        <v>4114492259.5300159</v>
       </c>
       <c r="E30" s="5">
-        <v>280</v>
+        <v>-57018744.210047364</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
-        <v>11</v>
+      <c r="B31" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C31" s="5">
-        <v>300</v>
+        <v>961939271.00999975</v>
       </c>
       <c r="D31" s="5">
-        <v>0</v>
+        <v>975690051.42999983</v>
       </c>
       <c r="E31" s="5">
-        <v>300</v>
+        <v>-13750780.42000002</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
-        <v>12</v>
+      <c r="B32" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C32" s="5">
         <v>0</v>
@@ -2312,8 +2971,8 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
-        <v>13</v>
+      <c r="B33" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C33" s="5">
         <v>0</v>
@@ -2326,8 +2985,8 @@
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
-        <v>14</v>
+      <c r="B34" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C34" s="5">
         <v>0</v>
@@ -2340,8 +2999,8 @@
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
-        <v>15</v>
+      <c r="B35" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C35" s="5">
         <v>0</v>
@@ -2354,367 +3013,17 @@
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
-        <v>5</v>
+      <c r="B36" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C36" s="5">
-        <v>24749826.379999999</v>
+        <v>10199114012.670002</v>
       </c>
       <c r="D36" s="5">
-        <v>24902085</v>
+        <v>10199115012.710001</v>
       </c>
       <c r="E36" s="5">
-        <v>-152258.62</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="5">
-        <v>24749826.379999999</v>
-      </c>
-      <c r="D37" s="5">
-        <v>24902085</v>
-      </c>
-      <c r="E37" s="5">
-        <v>-152258.62</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="5">
-        <v>111971812.90000001</v>
-      </c>
-      <c r="D38" s="5">
-        <v>94820875.549999997</v>
-      </c>
-      <c r="E38" s="5">
-        <v>17150937.350000009</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="5">
-        <v>111971812.90000001</v>
-      </c>
-      <c r="D39" s="5">
-        <v>94820875.549999997</v>
-      </c>
-      <c r="E39" s="5">
-        <v>17150937.350000009</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="5">
-        <v>111971812.90000001</v>
-      </c>
-      <c r="D40" s="5">
-        <v>94820875.549999997</v>
-      </c>
-      <c r="E40" s="5">
-        <v>17150937.350000009</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="5">
-        <v>44659934.850000001</v>
-      </c>
-      <c r="D41" s="5">
-        <v>61661453.57</v>
-      </c>
-      <c r="E41" s="5">
-        <v>-17001518.720000003</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="5">
-        <v>44659934.850000001</v>
-      </c>
-      <c r="D42" s="5">
-        <v>61661453.57</v>
-      </c>
-      <c r="E42" s="5">
-        <v>-17001518.720000003</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="5">
-        <v>20105299.149999999</v>
-      </c>
-      <c r="D43" s="5">
-        <v>36779274.830000006</v>
-      </c>
-      <c r="E43" s="5">
-        <v>-16673975.680000011</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="5">
-        <v>6278</v>
-      </c>
-      <c r="D44" s="5">
-        <v>228519.77000000002</v>
-      </c>
-      <c r="E44" s="5">
-        <v>-222241.77000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="5">
-        <v>19749309.849999998</v>
-      </c>
-      <c r="D45" s="5">
-        <v>36245026.799999997</v>
-      </c>
-      <c r="E45" s="5">
-        <v>-16495716.949999999</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="5">
-        <v>90</v>
-      </c>
-      <c r="D46" s="5">
-        <v>55022.76</v>
-      </c>
-      <c r="E46" s="5">
-        <v>-54932.76</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="5">
-        <v>690</v>
-      </c>
-      <c r="D47" s="5">
-        <v>2260</v>
-      </c>
-      <c r="E47" s="5">
-        <v>-1570</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="5">
-        <v>0</v>
-      </c>
-      <c r="D48" s="5">
-        <v>0</v>
-      </c>
-      <c r="E48" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="5">
-        <v>1300</v>
-      </c>
-      <c r="D49" s="5">
-        <v>1500</v>
-      </c>
-      <c r="E49" s="5">
-        <v>-200</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="5">
-        <v>347631.30000000005</v>
-      </c>
-      <c r="D50" s="5">
-        <v>246945.50000000003</v>
-      </c>
-      <c r="E50" s="5">
-        <v>100685.80000000002</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="5">
-        <v>24554635.700000003</v>
-      </c>
-      <c r="D51" s="5">
-        <v>24882178.739999998</v>
-      </c>
-      <c r="E51" s="5">
-        <v>-327543.03999999538</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" s="5">
-        <v>24554453.700000003</v>
-      </c>
-      <c r="D52" s="5">
-        <v>24447604.5</v>
-      </c>
-      <c r="E52" s="5">
-        <v>106849.20000000298</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="5">
-        <v>0</v>
-      </c>
-      <c r="D53" s="5">
-        <v>910</v>
-      </c>
-      <c r="E53" s="5">
-        <v>-910</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54" s="5">
-        <v>32</v>
-      </c>
-      <c r="D54" s="5">
-        <v>12568.46</v>
-      </c>
-      <c r="E54" s="5">
-        <v>-12536.46</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="5">
-        <v>0</v>
-      </c>
-      <c r="D55" s="5">
-        <v>420289.4</v>
-      </c>
-      <c r="E55" s="5">
-        <v>-420289.4</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" s="5">
-        <v>0</v>
-      </c>
-      <c r="D56" s="5">
-        <v>60</v>
-      </c>
-      <c r="E56" s="5">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="5">
-        <v>150</v>
-      </c>
-      <c r="D57" s="5">
-        <v>450</v>
-      </c>
-      <c r="E57" s="5">
-        <v>-300</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="5">
-        <v>0</v>
-      </c>
-      <c r="D58" s="5">
-        <v>276.38</v>
-      </c>
-      <c r="E58" s="5">
-        <v>-276.38</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" s="5">
-        <v>0</v>
-      </c>
-      <c r="D59" s="5">
-        <v>20</v>
-      </c>
-      <c r="E59" s="5">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C60" s="5">
-        <v>0</v>
-      </c>
-      <c r="D60" s="5">
-        <v>0</v>
-      </c>
-      <c r="E60" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="5">
-        <v>181384414.13000003</v>
-      </c>
-      <c r="D61" s="5">
-        <v>181384414.12</v>
-      </c>
-      <c r="E61" s="5">
-        <v>9.9999941885471344E-3</v>
+        <v>-1000.0400004386902</v>
       </c>
     </row>
   </sheetData>
@@ -2729,4 +3038,36 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>